<commit_message>
Added source to extrusion in bom
</commit_message>
<xml_diff>
--- a/Mechanical Assembly/BOM.xlsx
+++ b/Mechanical Assembly/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usherbrooke.sharepoint.com/sites/msteams_ec6dc4-quipe3/Documents partages/Équipe 3/Fichiers de projet/Documentation assemblage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flexo\Git\MixUS\Mechanical Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1020" documentId="8_{482AD615-B922-4F73-8925-C00A40D43CA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3AE8609-2575-4DB4-ABEA-BD34C744FE4F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D5D7F7-C9E6-4293-9E3A-9352C5E621BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="1" xr2:uid="{1A3A9EF6-5B5A-4F09-8571-A66E06D6AF83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{1A3A9EF6-5B5A-4F09-8571-A66E06D6AF83}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="199">
   <si>
     <t>Mecanic BOM: 100XXX</t>
   </si>
@@ -839,6 +839,9 @@
   </si>
   <si>
     <t>40x40x10_DC_Fan</t>
+  </si>
+  <si>
+    <t>https://openbuilds.com/</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1299,10 +1302,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1314,10 +1314,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1329,37 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1371,17 +1347,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2088,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9879C518-628C-43C9-AAEC-79C9102FF36C}">
   <dimension ref="B1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2100,7 +2106,8 @@
     <col min="4" max="4" width="23" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="9"/>
     <col min="6" max="6" width="26" style="9" customWidth="1"/>
-    <col min="7" max="9" width="11.5546875" style="9"/>
+    <col min="7" max="7" width="23.21875" style="9" customWidth="1"/>
+    <col min="8" max="9" width="11.5546875" style="9"/>
     <col min="10" max="10" width="55.6640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="28" style="9" customWidth="1"/>
     <col min="12" max="12" width="11.5546875" style="9"/>
@@ -2151,34 +2158,34 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="I4" s="87" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="I4" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
     </row>
     <row r="5" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="26" t="s">
@@ -2215,7 +2222,7 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="70" t="s">
         <v>76</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -2232,7 +2239,7 @@
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="70" t="s">
+      <c r="I7" s="69" t="s">
         <v>79</v>
       </c>
       <c r="J7" s="20" t="s">
@@ -2241,13 +2248,13 @@
       <c r="K7" s="20">
         <v>20</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="M7" s="82"/>
+      <c r="M7" s="91"/>
     </row>
     <row r="8" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="71"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="16" t="s">
         <v>82</v>
       </c>
@@ -2262,7 +2269,7 @@
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="72"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="19" t="s">
         <v>84</v>
       </c>
@@ -2277,7 +2284,7 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="16" t="s">
         <v>87</v>
       </c>
@@ -2292,7 +2299,7 @@
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="69" t="s">
         <v>88</v>
       </c>
       <c r="J9" s="20" t="s">
@@ -2302,13 +2309,13 @@
         <f xml:space="preserve"> 4 + (2*6)</f>
         <v>16</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="M9" s="82"/>
+      <c r="M9" s="91"/>
     </row>
     <row r="10" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="71"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="16" t="s">
         <v>90</v>
       </c>
@@ -2323,20 +2330,20 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="71"/>
+      <c r="I10" s="70"/>
       <c r="J10" s="16" t="s">
         <v>91</v>
       </c>
       <c r="K10" s="16">
         <v>3</v>
       </c>
-      <c r="L10" s="83" t="s">
+      <c r="L10" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="68"/>
+      <c r="M10" s="87"/>
     </row>
     <row r="11" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="72"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="19" t="s">
         <v>92</v>
       </c>
@@ -2351,7 +2358,7 @@
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="72"/>
+      <c r="I11" s="71"/>
       <c r="J11" s="58" t="s">
         <v>182</v>
       </c>
@@ -2366,7 +2373,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>95</v>
       </c>
       <c r="C12" s="20" t="s">
@@ -2383,7 +2390,7 @@
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="69" t="s">
         <v>93</v>
       </c>
       <c r="J12" s="25" t="s">
@@ -2392,13 +2399,13 @@
       <c r="K12" s="20">
         <v>16</v>
       </c>
-      <c r="L12" s="81" t="s">
+      <c r="L12" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="M12" s="82"/>
+      <c r="M12" s="91"/>
     </row>
     <row r="13" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="16" t="s">
         <v>101</v>
       </c>
@@ -2413,20 +2420,20 @@
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="71"/>
+      <c r="I13" s="70"/>
       <c r="J13" s="57" t="s">
         <v>97</v>
       </c>
       <c r="K13" s="16">
         <v>20</v>
       </c>
-      <c r="L13" s="83" t="s">
+      <c r="L13" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="M13" s="68"/>
+      <c r="M13" s="87"/>
     </row>
     <row r="14" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="71"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="16" t="s">
         <v>103</v>
       </c>
@@ -2441,20 +2448,20 @@
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="71"/>
+      <c r="I14" s="70"/>
       <c r="J14" s="57" t="s">
         <v>100</v>
       </c>
       <c r="K14" s="16">
         <v>150</v>
       </c>
-      <c r="L14" s="83" t="s">
+      <c r="L14" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="M14" s="68"/>
+      <c r="M14" s="87"/>
     </row>
     <row r="15" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="71"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="16" t="s">
         <v>104</v>
       </c>
@@ -2469,20 +2476,20 @@
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="71"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="57" t="s">
         <v>102</v>
       </c>
       <c r="K15" s="16">
         <v>3</v>
       </c>
-      <c r="L15" s="83" t="s">
+      <c r="L15" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="68"/>
+      <c r="M15" s="87"/>
     </row>
     <row r="16" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="16" t="s">
         <v>105</v>
       </c>
@@ -2497,7 +2504,7 @@
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="71"/>
+      <c r="I16" s="70"/>
       <c r="J16" s="57" t="s">
         <v>180</v>
       </c>
@@ -2513,7 +2520,7 @@
       <c r="N16" s="67"/>
     </row>
     <row r="17" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="16" t="s">
         <v>98</v>
       </c>
@@ -2528,20 +2535,20 @@
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="71"/>
+      <c r="I17" s="70"/>
       <c r="J17" s="57" t="s">
         <v>179</v>
       </c>
       <c r="K17" s="18">
         <v>78</v>
       </c>
-      <c r="L17" s="83" t="s">
+      <c r="L17" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="M17" s="68"/>
+      <c r="M17" s="87"/>
     </row>
     <row r="18" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="71"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="16" t="s">
         <v>178</v>
       </c>
@@ -2554,20 +2561,20 @@
       <c r="F18" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="72"/>
+      <c r="I18" s="71"/>
       <c r="J18" s="22" t="s">
         <v>181</v>
       </c>
       <c r="K18" s="22">
         <v>24</v>
       </c>
-      <c r="L18" s="84" t="s">
+      <c r="L18" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="M18" s="69"/>
+      <c r="M18" s="89"/>
     </row>
     <row r="19" spans="2:13" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="16" t="s">
         <v>156</v>
       </c>
@@ -2582,7 +2589,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="71"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="16" t="s">
         <v>157</v>
       </c>
@@ -2597,7 +2604,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="71"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="16" t="s">
         <v>158</v>
       </c>
@@ -2612,7 +2619,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="71"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="16" t="s">
         <v>106</v>
       </c>
@@ -2629,8 +2636,8 @@
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
-      <c r="C23" s="79" t="s">
+      <c r="B23" s="70"/>
+      <c r="C23" s="73" t="s">
         <v>107</v>
       </c>
       <c r="D23" s="16" t="s">
@@ -2639,37 +2646,37 @@
       <c r="E23" s="16">
         <v>1</v>
       </c>
-      <c r="F23" s="89" t="s">
+      <c r="F23" s="80" t="s">
         <v>108</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="72"/>
-      <c r="C24" s="80"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="79"/>
       <c r="D24" s="19" t="s">
         <v>110</v>
       </c>
       <c r="E24" s="19">
         <v>1</v>
       </c>
-      <c r="F24" s="90"/>
+      <c r="F24" s="81"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="87" t="s">
+      <c r="I24" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
     </row>
     <row r="25" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="72" t="s">
         <v>112</v>
       </c>
       <c r="D25" s="20" t="s">
@@ -2678,27 +2685,27 @@
       <c r="E25" s="20">
         <v>1</v>
       </c>
-      <c r="F25" s="95" t="s">
+      <c r="F25" s="74" t="s">
         <v>113</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
     </row>
     <row r="26" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="71"/>
-      <c r="C26" s="79"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="16">
         <v>1</v>
       </c>
-      <c r="F26" s="92"/>
+      <c r="F26" s="75"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="26" t="s">
@@ -2718,7 +2725,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="72"/>
+      <c r="B27" s="71"/>
       <c r="C27" s="19" t="s">
         <v>119</v>
       </c>
@@ -2733,7 +2740,7 @@
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="70" t="s">
+      <c r="I27" s="69" t="s">
         <v>114</v>
       </c>
       <c r="J27" s="52" t="s">
@@ -2750,10 +2757,10 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="72" t="s">
         <v>123</v>
       </c>
       <c r="D28" s="20" t="s">
@@ -2762,12 +2769,14 @@
       <c r="E28" s="21">
         <v>3</v>
       </c>
-      <c r="F28" s="91" t="s">
+      <c r="F28" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="96" t="s">
+        <v>198</v>
+      </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="72"/>
+      <c r="I28" s="71"/>
       <c r="J28" s="53" t="s">
         <v>116</v>
       </c>
@@ -2782,18 +2791,18 @@
       </c>
     </row>
     <row r="29" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="76"/>
-      <c r="C29" s="79"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="73"/>
       <c r="D29" s="16" t="s">
         <v>126</v>
       </c>
       <c r="E29" s="16">
         <v>2</v>
       </c>
-      <c r="F29" s="92"/>
-      <c r="G29" s="12"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="70"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="70" t="s">
+      <c r="I29" s="69" t="s">
         <v>120</v>
       </c>
       <c r="J29" s="54" t="s">
@@ -2810,8 +2819,8 @@
       </c>
     </row>
     <row r="30" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="76"/>
-      <c r="C30" s="93" t="s">
+      <c r="B30" s="77"/>
+      <c r="C30" s="83" t="s">
         <v>128</v>
       </c>
       <c r="D30" s="18" t="s">
@@ -2823,9 +2832,9 @@
       <c r="F30" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="70"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="72"/>
+      <c r="I30" s="71"/>
       <c r="J30" s="53" t="s">
         <v>125</v>
       </c>
@@ -2840,8 +2849,8 @@
       </c>
     </row>
     <row r="31" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="76"/>
-      <c r="C31" s="93"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="18" t="s">
         <v>130</v>
       </c>
@@ -2851,9 +2860,9 @@
       <c r="F31" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G31" s="12"/>
+      <c r="G31" s="70"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="70" t="s">
+      <c r="I31" s="69" t="s">
         <v>127</v>
       </c>
       <c r="J31" s="25" t="s">
@@ -2870,8 +2879,8 @@
       </c>
     </row>
     <row r="32" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="77"/>
-      <c r="C32" s="94"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="84"/>
       <c r="D32" s="22" t="s">
         <v>132</v>
       </c>
@@ -2881,9 +2890,9 @@
       <c r="F32" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="12"/>
+      <c r="G32" s="70"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="71"/>
+      <c r="I32" s="70"/>
       <c r="J32" s="57" t="s">
         <v>162</v>
       </c>
@@ -2898,7 +2907,7 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="69" t="s">
         <v>133</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -2915,7 +2924,7 @@
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="71"/>
+      <c r="I33" s="70"/>
       <c r="J33" s="52" t="s">
         <v>164</v>
       </c>
@@ -2930,7 +2939,7 @@
       </c>
     </row>
     <row r="34" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="72"/>
+      <c r="B34" s="71"/>
       <c r="C34" s="19" t="s">
         <v>136</v>
       </c>
@@ -2945,7 +2954,7 @@
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="71"/>
+      <c r="I34" s="70"/>
       <c r="J34" s="52" t="s">
         <v>131</v>
       </c>
@@ -2955,12 +2964,12 @@
       <c r="L34" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="M34" s="68" t="s">
+      <c r="M34" s="87" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="69" t="s">
         <v>166</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -2977,7 +2986,7 @@
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="71"/>
+      <c r="I35" s="70"/>
       <c r="J35" s="52" t="s">
         <v>153</v>
       </c>
@@ -2987,10 +2996,10 @@
       <c r="L35" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="M35" s="68"/>
+      <c r="M35" s="87"/>
     </row>
     <row r="36" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="71"/>
+      <c r="B36" s="70"/>
       <c r="C36" s="16" t="s">
         <v>168</v>
       </c>
@@ -3005,7 +3014,7 @@
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="72"/>
+      <c r="I36" s="71"/>
       <c r="J36" s="53" t="s">
         <v>165</v>
       </c>
@@ -3015,10 +3024,10 @@
       <c r="L36" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="M36" s="69"/>
+      <c r="M36" s="89"/>
     </row>
     <row r="37" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="71"/>
+      <c r="B37" s="70"/>
       <c r="C37" s="16" t="s">
         <v>169</v>
       </c>
@@ -3031,7 +3040,7 @@
       <c r="F37" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="I37" s="70" t="s">
+      <c r="I37" s="69" t="s">
         <v>135</v>
       </c>
       <c r="J37" s="25" t="s">
@@ -3048,7 +3057,7 @@
       </c>
     </row>
     <row r="38" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="72"/>
+      <c r="B38" s="71"/>
       <c r="C38" s="19" t="s">
         <v>170</v>
       </c>
@@ -3061,7 +3070,7 @@
       <c r="F38" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="I38" s="71"/>
+      <c r="I38" s="70"/>
       <c r="J38" s="60" t="s">
         <v>155</v>
       </c>
@@ -3076,10 +3085,10 @@
       </c>
     </row>
     <row r="39" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="78" t="s">
+      <c r="C39" s="72" t="s">
         <v>172</v>
       </c>
       <c r="D39" s="20" t="s">
@@ -3091,7 +3100,7 @@
       <c r="F39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="I39" s="71"/>
+      <c r="I39" s="70"/>
       <c r="J39" s="59" t="s">
         <v>137</v>
       </c>
@@ -3106,8 +3115,8 @@
       </c>
     </row>
     <row r="40" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="71"/>
-      <c r="C40" s="79"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="73"/>
       <c r="D40" s="16" t="s">
         <v>174</v>
       </c>
@@ -3117,7 +3126,7 @@
       <c r="F40" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I40" s="72"/>
+      <c r="I40" s="71"/>
       <c r="J40" s="61" t="s">
         <v>197</v>
       </c>
@@ -3132,8 +3141,8 @@
       </c>
     </row>
     <row r="41" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="71"/>
-      <c r="C41" s="79" t="s">
+      <c r="B41" s="70"/>
+      <c r="C41" s="73" t="s">
         <v>175</v>
       </c>
       <c r="D41" s="16" t="s">
@@ -3150,8 +3159,8 @@
       <c r="M41" s="15"/>
     </row>
     <row r="42" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="71"/>
-      <c r="C42" s="79"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="73"/>
       <c r="D42" s="16" t="s">
         <v>174</v>
       </c>
@@ -3163,8 +3172,8 @@
       </c>
     </row>
     <row r="43" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="71"/>
-      <c r="C43" s="79" t="s">
+      <c r="B43" s="70"/>
+      <c r="C43" s="73" t="s">
         <v>176</v>
       </c>
       <c r="D43" s="16" t="s">
@@ -3180,8 +3189,8 @@
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="71"/>
-      <c r="C44" s="79"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="73"/>
       <c r="D44" s="16" t="s">
         <v>110</v>
       </c>
@@ -3195,8 +3204,8 @@
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="71"/>
-      <c r="C45" s="79" t="s">
+      <c r="B45" s="70"/>
+      <c r="C45" s="73" t="s">
         <v>177</v>
       </c>
       <c r="D45" s="16" t="s">
@@ -3210,17 +3219,17 @@
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="88" t="s">
+      <c r="I45" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="J45" s="88"/>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
     </row>
     <row r="46" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="72"/>
-      <c r="C46" s="80"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="79"/>
       <c r="D46" s="19" t="s">
         <v>110</v>
       </c>
@@ -3232,11 +3241,11 @@
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="88"/>
-      <c r="J46" s="88"/>
-      <c r="K46" s="88"/>
-      <c r="L46" s="88"/>
-      <c r="M46" s="88"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="68"/>
+      <c r="K46" s="68"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="68"/>
     </row>
     <row r="47" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
@@ -3270,7 +3279,7 @@
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="70" t="s">
+      <c r="I48" s="69" t="s">
         <v>111</v>
       </c>
       <c r="J48" s="16" t="s">
@@ -3287,16 +3296,16 @@
       </c>
     </row>
     <row r="49" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="88" t="s">
+      <c r="B49" s="68" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
-      <c r="E49" s="88"/>
-      <c r="F49" s="88"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="68"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="71"/>
+      <c r="I49" s="70"/>
       <c r="J49" s="16" t="s">
         <v>161</v>
       </c>
@@ -3311,14 +3320,14 @@
       </c>
     </row>
     <row r="50" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="88"/>
-      <c r="C50" s="88"/>
-      <c r="D50" s="88"/>
-      <c r="E50" s="88"/>
-      <c r="F50" s="88"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="68"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="71"/>
+      <c r="I50" s="70"/>
       <c r="J50" s="16" t="s">
         <v>143</v>
       </c>
@@ -3340,13 +3349,13 @@
       <c r="D51" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="E51" s="85" t="s">
+      <c r="E51" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="F51" s="86"/>
+      <c r="F51" s="93"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="71"/>
+      <c r="I51" s="70"/>
       <c r="J51" s="16" t="s">
         <v>152</v>
       </c>
@@ -3361,7 +3370,7 @@
       </c>
     </row>
     <row r="52" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="76" t="s">
         <v>193</v>
       </c>
       <c r="C52" s="54" t="s">
@@ -3370,13 +3379,13 @@
       <c r="D52" s="54">
         <v>8</v>
       </c>
-      <c r="E52" s="81" t="s">
+      <c r="E52" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="F52" s="82"/>
+      <c r="F52" s="91"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="71"/>
+      <c r="I52" s="70"/>
       <c r="J52" s="16" t="s">
         <v>144</v>
       </c>
@@ -3391,18 +3400,18 @@
       </c>
     </row>
     <row r="53" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="71"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="52" t="s">
         <v>191</v>
       </c>
       <c r="D53" s="52">
         <v>6</v>
       </c>
-      <c r="E53" s="83"/>
-      <c r="F53" s="68"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="87"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="72"/>
+      <c r="I53" s="71"/>
       <c r="J53" s="19" t="s">
         <v>183</v>
       </c>
@@ -3418,18 +3427,18 @@
       </c>
     </row>
     <row r="54" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="72"/>
+      <c r="B54" s="71"/>
       <c r="C54" s="53" t="s">
         <v>192</v>
       </c>
       <c r="D54" s="53">
         <v>5</v>
       </c>
-      <c r="E54" s="84"/>
-      <c r="F54" s="69"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="89"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="70" t="s">
+      <c r="I54" s="69" t="s">
         <v>76</v>
       </c>
       <c r="J54" s="20" t="s">
@@ -3446,20 +3455,20 @@
       </c>
     </row>
     <row r="55" spans="2:13" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="75" t="s">
+      <c r="B55" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="C55" s="78" t="s">
+      <c r="C55" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="78">
+      <c r="D55" s="72">
         <v>6</v>
       </c>
-      <c r="E55" s="81" t="s">
+      <c r="E55" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="F55" s="82"/>
-      <c r="I55" s="71"/>
+      <c r="F55" s="91"/>
+      <c r="I55" s="70"/>
       <c r="J55" s="16" t="s">
         <v>146</v>
       </c>
@@ -3474,14 +3483,14 @@
       </c>
     </row>
     <row r="56" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="76"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="68"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="87"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="71"/>
+      <c r="I56" s="70"/>
       <c r="J56" s="16" t="s">
         <v>148</v>
       </c>
@@ -3496,12 +3505,12 @@
       </c>
     </row>
     <row r="57" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="77"/>
-      <c r="C57" s="80"/>
-      <c r="D57" s="80"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="69"/>
-      <c r="I57" s="72"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="89"/>
+      <c r="I57" s="71"/>
       <c r="J57" s="44" t="s">
         <v>149</v>
       </c>
@@ -3516,20 +3525,20 @@
       </c>
     </row>
     <row r="58" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="75" t="s">
+      <c r="B58" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C58" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="D58" s="78">
+      <c r="D58" s="72">
         <v>2</v>
       </c>
-      <c r="E58" s="81" t="s">
+      <c r="E58" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="F58" s="82"/>
-      <c r="I58" s="73" t="s">
+      <c r="F58" s="91"/>
+      <c r="I58" s="94" t="s">
         <v>139</v>
       </c>
       <c r="J58" s="25" t="s">
@@ -3546,12 +3555,12 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="76"/>
-      <c r="C59" s="79"/>
-      <c r="D59" s="79"/>
-      <c r="E59" s="83"/>
-      <c r="F59" s="68"/>
-      <c r="I59" s="74"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="87"/>
+      <c r="I59" s="95"/>
       <c r="J59" s="45" t="s">
         <v>150</v>
       </c>
@@ -3566,11 +3575,11 @@
       </c>
     </row>
     <row r="60" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="77"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="80"/>
-      <c r="E60" s="84"/>
-      <c r="F60" s="69"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="88"/>
+      <c r="F60" s="89"/>
       <c r="I60" s="39" t="s">
         <v>95</v>
       </c>
@@ -3588,42 +3597,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B39:B46"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I18"/>
-    <mergeCell ref="B12:B24"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="I4:M5"/>
-    <mergeCell ref="I24:M25"/>
-    <mergeCell ref="I45:M46"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B7:B11"/>
+  <mergeCells count="55">
+    <mergeCell ref="G28:G32"/>
+    <mergeCell ref="I54:I57"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I31:I36"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I48:I53"/>
+    <mergeCell ref="I37:I40"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="D58:D60"/>
@@ -3635,14 +3617,42 @@
     <mergeCell ref="D55:D57"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="E55:F57"/>
+    <mergeCell ref="I45:M46"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="M34:M36"/>
-    <mergeCell ref="I54:I57"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I31:I36"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I48:I53"/>
-    <mergeCell ref="I37:I40"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I18"/>
+    <mergeCell ref="B12:B24"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="I4:M5"/>
+    <mergeCell ref="I24:M25"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B39:B46"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B33:B34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" xr:uid="{5172537A-33E6-4E0C-ABA2-601DC871E734}"/>
@@ -3690,14 +3700,30 @@
     <hyperlink ref="M58" r:id="rId43" xr:uid="{E79AA6E2-6FF2-45A7-95C6-7FE3ECBD7283}"/>
     <hyperlink ref="L40" r:id="rId44" xr:uid="{AC4662CD-1751-42AB-95E7-FA218452C7DD}"/>
     <hyperlink ref="M40" r:id="rId45" xr:uid="{59C9229B-DBC7-4429-857D-B266A2F51EF3}"/>
+    <hyperlink ref="G28" r:id="rId46" xr:uid="{8166A8F4-8BBA-45E3-99A0-4296F9D21E06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId46"/>
-  <legacyDrawing r:id="rId47"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId47"/>
+  <legacyDrawing r:id="rId48"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BBA214270DBFC542AB0F9FF94914DBEB" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="8e3cbac9c8e03cdd177f9f20636d8ffb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0adf8362-02b7-44e7-8c4c-be15739613ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1b9dad6dd0c16a8d60794080e653965" ns2:_="">
     <xsd:import namespace="0adf8362-02b7-44e7-8c4c-be15739613ed"/>
@@ -3867,22 +3893,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9CFBF4-672A-45B6-AA3F-87CBA6A65A46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0adf8362-02b7-44e7-8c4c-be15739613ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7D04AC3-C0AB-438E-9115-687AE1BBC194}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5C6B067-28F7-4073-B288-E9A9BFFEA03C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3898,28 +3933,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7D04AC3-C0AB-438E-9115-687AE1BBC194}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9CFBF4-672A-45B6-AA3F-87CBA6A65A46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0adf8362-02b7-44e7-8c4c-be15739613ed"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>